<commit_message>
datasource update - additional changes
</commit_message>
<xml_diff>
--- a/PowerShell/Projekt - Deployment Script/Version 1/DeploymentAppConfig_v1.xlsx
+++ b/PowerShell/Projekt - Deployment Script/Version 1/DeploymentAppConfig_v1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="156" windowWidth="24792" windowHeight="12288"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="24795" windowHeight="12285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PortalOrdner" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>/DEV99</t>
   </si>
@@ -87,6 +87,24 @@
   </si>
   <si>
     <t>PortalPath</t>
+  </si>
+  <si>
+    <t>EnvServer</t>
+  </si>
+  <si>
+    <t>sv-rc-310\MSSQLSERVER_TEST</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>https://sv-rc-310.rega.local/Reports</t>
+  </si>
+  <si>
+    <t>Env</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -459,14 +477,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -572,10 +590,10 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -625,25 +643,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="33.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="38.25" customWidth="1"/>
+    <col min="3" max="3" width="27.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>